<commit_message>
added tmp creation functions logic, need to create view interface
</commit_message>
<xml_diff>
--- a/templates/KTI_Discharge_Invoice.xlsx
+++ b/templates/KTI_Discharge_Invoice.xlsx
@@ -8,34 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F826C743-C1C6-4206-8D4C-B96515D58305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B19E45-A9FE-455D-A351-085F60A589E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42540" yWindow="5258" windowWidth="14385" windowHeight="7484" tabRatio="896" activeTab="1" xr2:uid="{A5E11D55-FD63-4C1B-A2BC-73BE53B894FE}"/>
+    <workbookView xWindow="-26978" yWindow="-98" windowWidth="27076" windowHeight="16395" tabRatio="896" activeTab="1" xr2:uid="{A5E11D55-FD63-4C1B-A2BC-73BE53B894FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Б.Нагаева хранение ТРК" sheetId="71" r:id="rId1"/>
-    <sheet name="Б.Нагаева выгрузка ТРК 010623" sheetId="70" r:id="rId2"/>
+    <sheet name="Invoice_discharge" sheetId="70" r:id="rId2"/>
     <sheet name="Б.Нагаева хранениеМСИ " sheetId="77" r:id="rId3"/>
     <sheet name="Б. Нагаева выгрузка МСИ010623" sheetId="69" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="Инвойс_всего">'Б.Нагаева выгрузка ТРК 010623'!$J$40</definedName>
-    <definedName name="Инвойс_всего_п">'Б.Нагаева выгрузка ТРК 010623'!$H$107</definedName>
-    <definedName name="Инвойс_выгрузка_дата">'Б.Нагаева выгрузка ТРК 010623'!$C$17</definedName>
-    <definedName name="Инвойс_дата_п">'Б.Нагаева выгрузка ТРК 010623'!$J$78</definedName>
-    <definedName name="Инвойс_компания">'Б.Нагаева выгрузка ТРК 010623'!$C$10</definedName>
-    <definedName name="Инвойс_компания_п">'Б.Нагаева выгрузка ТРК 010623'!$C$78</definedName>
-    <definedName name="Инвойс_контракт">'Б.Нагаева выгрузка ТРК 010623'!$C$12</definedName>
-    <definedName name="Инвойс_контракт_п">'Б.Нагаева выгрузка ТРК 010623'!$C$80</definedName>
-    <definedName name="Инвойс_массив">'Б.Нагаева выгрузка ТРК 010623'!$B$26</definedName>
-    <definedName name="Инвойс_массив_п">'Б.Нагаева выгрузка ТРК 010623'!$B$93</definedName>
-    <definedName name="Инвойс_номер">'Б.Нагаева выгрузка ТРК 010623'!$E$8</definedName>
-    <definedName name="Инвойс_номер_п">'Б.Нагаева выгрузка ТРК 010623'!$E$76</definedName>
-    <definedName name="Инвойс_соглашение">'Б.Нагаева выгрузка ТРК 010623'!$C$21</definedName>
-    <definedName name="Инвойс_соглашение_п">'Б.Нагаева выгрузка ТРК 010623'!$C$88</definedName>
-    <definedName name="Инвойс_транспорт">'Б.Нагаева выгрузка ТРК 010623'!$C$19</definedName>
-    <definedName name="Инвойс_транспорт_п">'Б.Нагаева выгрузка ТРК 010623'!$C$86</definedName>
-    <definedName name="Инвойсс_выгрузка_дата_п">'Б.Нагаева выгрузка ТРК 010623'!$C$84</definedName>
+    <definedName name="Инвойс_всего">Invoice_discharge!$J$40</definedName>
+    <definedName name="Инвойс_всего_п">Invoice_discharge!$H$107</definedName>
+    <definedName name="Инвойс_выгрузка_дата">Invoice_discharge!$C$17</definedName>
+    <definedName name="Инвойс_дата">Invoice_discharge!$J$10</definedName>
+    <definedName name="Инвойс_дата_п">Invoice_discharge!$J$78</definedName>
+    <definedName name="Инвойс_компания">Invoice_discharge!$C$10</definedName>
+    <definedName name="Инвойс_компания_п">Invoice_discharge!$C$78</definedName>
+    <definedName name="Инвойс_контракт">Invoice_discharge!$C$12</definedName>
+    <definedName name="Инвойс_контракт_п">Invoice_discharge!$C$80</definedName>
+    <definedName name="Инвойс_массив">Invoice_discharge!$B$26</definedName>
+    <definedName name="Инвойс_массив_п">Invoice_discharge!$B$93</definedName>
+    <definedName name="Инвойс_номер">Invoice_discharge!$E$8</definedName>
+    <definedName name="Инвойс_номер_п">Invoice_discharge!$E$76</definedName>
+    <definedName name="Инвойс_соглашение">Invoice_discharge!$C$21</definedName>
+    <definedName name="Инвойс_соглашение_п">Invoice_discharge!$C$88</definedName>
+    <definedName name="Инвойс_транспорт">Invoice_discharge!$C$19</definedName>
+    <definedName name="Инвойс_транспорт_п">Invoice_discharge!$C$86</definedName>
+    <definedName name="Инвойсс_выгрузка_дата_п">Invoice_discharge!$C$84</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1004,6 +1005,30 @@
     <xf numFmtId="169" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1014,29 +1039,11 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1068,9 +1075,6 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="170" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1079,9 +1083,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2379,15 +2380,15 @@
   <sheetData>
     <row r="1" spans="2:11" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:11" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="127" t="s">
+      <c r="C2" s="135" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="127"/>
-      <c r="E2" s="127"/>
-      <c r="F2" s="127"/>
-      <c r="G2" s="127"/>
-      <c r="H2" s="127"/>
-      <c r="I2" s="127"/>
+      <c r="D2" s="135"/>
+      <c r="E2" s="135"/>
+      <c r="F2" s="135"/>
+      <c r="G2" s="135"/>
+      <c r="H2" s="135"/>
+      <c r="I2" s="135"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
@@ -2405,39 +2406,39 @@
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C4" s="128" t="s">
+      <c r="C4" s="136" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="128"/>
-      <c r="E4" s="128"/>
-      <c r="F4" s="128"/>
-      <c r="G4" s="128"/>
-      <c r="H4" s="128"/>
-      <c r="I4" s="128"/>
-      <c r="J4" s="128"/>
+      <c r="D4" s="136"/>
+      <c r="E4" s="136"/>
+      <c r="F4" s="136"/>
+      <c r="G4" s="136"/>
+      <c r="H4" s="136"/>
+      <c r="I4" s="136"/>
+      <c r="J4" s="136"/>
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C5" s="128" t="s">
+      <c r="C5" s="136" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="128"/>
-      <c r="E5" s="128"/>
-      <c r="F5" s="128"/>
-      <c r="G5" s="128"/>
-      <c r="H5" s="126"/>
-      <c r="I5" s="126"/>
-      <c r="J5" s="126"/>
+      <c r="D5" s="136"/>
+      <c r="E5" s="136"/>
+      <c r="F5" s="136"/>
+      <c r="G5" s="136"/>
+      <c r="H5" s="134"/>
+      <c r="I5" s="134"/>
+      <c r="J5" s="134"/>
       <c r="K5" s="3"/>
     </row>
     <row r="6" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
-      <c r="D6" s="125"/>
-      <c r="E6" s="125"/>
-      <c r="F6" s="125"/>
-      <c r="H6" s="126"/>
-      <c r="I6" s="126"/>
-      <c r="J6" s="126"/>
+      <c r="D6" s="133"/>
+      <c r="E6" s="133"/>
+      <c r="F6" s="133"/>
+      <c r="H6" s="134"/>
+      <c r="I6" s="134"/>
+      <c r="J6" s="134"/>
       <c r="K6" s="3"/>
     </row>
     <row r="7" spans="2:11" ht="9.6" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2471,10 +2472,10 @@
       <c r="I10" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="J10" s="129">
+      <c r="J10" s="125">
         <v>45107</v>
       </c>
-      <c r="K10" s="129"/>
+      <c r="K10" s="125"/>
     </row>
     <row r="11" spans="2:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B11" s="8"/>
@@ -2603,24 +2604,24 @@
     </row>
     <row r="24" spans="2:17" ht="10.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="2:17" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B25" s="130" t="s">
+      <c r="B25" s="126" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="130"/>
-      <c r="D25" s="130"/>
-      <c r="E25" s="131"/>
-      <c r="F25" s="132" t="s">
+      <c r="C25" s="126"/>
+      <c r="D25" s="126"/>
+      <c r="E25" s="127"/>
+      <c r="F25" s="128" t="s">
         <v>25</v>
       </c>
-      <c r="G25" s="131"/>
-      <c r="H25" s="133" t="s">
+      <c r="G25" s="127"/>
+      <c r="H25" s="129" t="s">
         <v>26</v>
       </c>
-      <c r="I25" s="134"/>
-      <c r="J25" s="135" t="s">
+      <c r="I25" s="130"/>
+      <c r="J25" s="131" t="s">
         <v>12</v>
       </c>
-      <c r="K25" s="136"/>
+      <c r="K25" s="132"/>
     </row>
     <row r="26" spans="2:17" ht="13.9" x14ac:dyDescent="0.4">
       <c r="B26" s="37" t="s">
@@ -2995,17 +2996,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="J25:K25"/>
     <mergeCell ref="D6:F6"/>
     <mergeCell ref="H6:J6"/>
     <mergeCell ref="C2:I2"/>
     <mergeCell ref="C4:J4"/>
     <mergeCell ref="C5:G5"/>
     <mergeCell ref="H5:J5"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J25:K25"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="94" orientation="portrait" r:id="rId1"/>
@@ -3025,8 +3026,8 @@
   </sheetPr>
   <dimension ref="B1:Q122"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A69" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72:G72"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A63" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="J75" sqref="J75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -3896,19 +3897,19 @@
       <c r="C5" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="147"/>
-      <c r="I5" s="147"/>
-      <c r="J5" s="147"/>
+      <c r="H5" s="137"/>
+      <c r="I5" s="137"/>
+      <c r="J5" s="137"/>
       <c r="K5" s="63"/>
     </row>
     <row r="6" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="63"/>
-      <c r="D6" s="152"/>
-      <c r="E6" s="152"/>
-      <c r="F6" s="152"/>
-      <c r="H6" s="147"/>
-      <c r="I6" s="147"/>
-      <c r="J6" s="147"/>
+      <c r="D6" s="138"/>
+      <c r="E6" s="138"/>
+      <c r="F6" s="138"/>
+      <c r="H6" s="137"/>
+      <c r="I6" s="137"/>
+      <c r="J6" s="137"/>
       <c r="K6" s="63"/>
     </row>
     <row r="7" spans="2:11" ht="9.6" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -3942,10 +3943,10 @@
       <c r="I10" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="J10" s="129">
+      <c r="J10" s="125">
         <v>45079</v>
       </c>
-      <c r="K10" s="129"/>
+      <c r="K10" s="125"/>
     </row>
     <row r="11" spans="2:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B11" s="8"/>
@@ -4060,21 +4061,21 @@
     </row>
     <row r="23" spans="2:17" ht="10.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="24" spans="2:17" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B24" s="138" t="s">
+      <c r="B24" s="140" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="138"/>
-      <c r="D24" s="138"/>
-      <c r="E24" s="138"/>
-      <c r="F24" s="139"/>
-      <c r="G24" s="141" t="s">
+      <c r="C24" s="140"/>
+      <c r="D24" s="140"/>
+      <c r="E24" s="140"/>
+      <c r="F24" s="141"/>
+      <c r="G24" s="143" t="s">
         <v>23</v>
       </c>
-      <c r="H24" s="138"/>
-      <c r="I24" s="135" t="s">
+      <c r="H24" s="140"/>
+      <c r="I24" s="131" t="s">
         <v>12</v>
       </c>
-      <c r="J24" s="140"/>
+      <c r="J24" s="142"/>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B25" s="10"/>
@@ -4280,15 +4281,15 @@
       <c r="I46" s="69"/>
     </row>
     <row r="70" spans="2:11" ht="30.4" x14ac:dyDescent="0.4">
-      <c r="C70" s="149" t="s">
+      <c r="C70" s="150" t="s">
         <v>46</v>
       </c>
-      <c r="D70" s="149"/>
-      <c r="E70" s="149"/>
-      <c r="F70" s="149"/>
-      <c r="G70" s="149"/>
-      <c r="H70" s="149"/>
-      <c r="I70" s="149"/>
+      <c r="D70" s="150"/>
+      <c r="E70" s="150"/>
+      <c r="F70" s="150"/>
+      <c r="G70" s="150"/>
+      <c r="H70" s="150"/>
+      <c r="I70" s="150"/>
       <c r="J70" s="61"/>
       <c r="K70" s="61"/>
     </row>
@@ -4306,44 +4307,44 @@
       <c r="K71" s="94"/>
     </row>
     <row r="72" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="C72" s="150" t="s">
+      <c r="C72" s="151" t="s">
         <v>48</v>
       </c>
-      <c r="D72" s="150"/>
-      <c r="E72" s="150"/>
-      <c r="F72" s="150"/>
-      <c r="G72" s="150"/>
-      <c r="H72" s="151"/>
-      <c r="I72" s="151"/>
-      <c r="J72" s="151"/>
+      <c r="D72" s="151"/>
+      <c r="E72" s="151"/>
+      <c r="F72" s="151"/>
+      <c r="G72" s="151"/>
+      <c r="H72" s="152"/>
+      <c r="I72" s="152"/>
+      <c r="J72" s="152"/>
       <c r="K72" s="95"/>
     </row>
     <row r="73" spans="2:11" ht="15" x14ac:dyDescent="0.4">
       <c r="B73" s="63"/>
-      <c r="C73" s="150" t="s">
+      <c r="C73" s="151" t="s">
         <v>49</v>
       </c>
-      <c r="D73" s="150"/>
-      <c r="E73" s="150"/>
-      <c r="F73" s="150"/>
-      <c r="G73" s="150"/>
-      <c r="H73" s="151"/>
-      <c r="I73" s="151"/>
-      <c r="J73" s="151"/>
+      <c r="D73" s="151"/>
+      <c r="E73" s="151"/>
+      <c r="F73" s="151"/>
+      <c r="G73" s="151"/>
+      <c r="H73" s="152"/>
+      <c r="I73" s="152"/>
+      <c r="J73" s="152"/>
       <c r="K73" s="95"/>
     </row>
     <row r="74" spans="2:11" ht="15" x14ac:dyDescent="0.4">
       <c r="B74" s="63"/>
-      <c r="C74" s="128" t="s">
+      <c r="C74" s="136" t="s">
         <v>3</v>
       </c>
-      <c r="D74" s="128"/>
-      <c r="E74" s="128"/>
-      <c r="F74" s="128"/>
-      <c r="G74" s="128"/>
-      <c r="H74" s="147"/>
-      <c r="I74" s="147"/>
-      <c r="J74" s="147"/>
+      <c r="D74" s="136"/>
+      <c r="E74" s="136"/>
+      <c r="F74" s="136"/>
+      <c r="G74" s="136"/>
+      <c r="H74" s="137"/>
+      <c r="I74" s="137"/>
+      <c r="J74" s="137"/>
       <c r="K74" s="63"/>
     </row>
     <row r="76" spans="2:11" ht="15" x14ac:dyDescent="0.4">
@@ -4375,10 +4376,10 @@
       <c r="I78" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="J78" s="148">
+      <c r="J78" s="149">
         <v>45033</v>
       </c>
-      <c r="K78" s="148"/>
+      <c r="K78" s="149"/>
     </row>
     <row r="79" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B79" s="8"/>
@@ -4497,21 +4498,21 @@
       <c r="J90" s="121"/>
     </row>
     <row r="91" spans="2:11" ht="19.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B91" s="142" t="s">
+      <c r="B91" s="144" t="s">
         <v>75</v>
       </c>
-      <c r="C91" s="142"/>
-      <c r="D91" s="142"/>
-      <c r="E91" s="142"/>
-      <c r="F91" s="143"/>
-      <c r="G91" s="144" t="s">
+      <c r="C91" s="144"/>
+      <c r="D91" s="144"/>
+      <c r="E91" s="144"/>
+      <c r="F91" s="145"/>
+      <c r="G91" s="146" t="s">
         <v>76</v>
       </c>
-      <c r="H91" s="146"/>
-      <c r="I91" s="144" t="s">
+      <c r="H91" s="148"/>
+      <c r="I91" s="146" t="s">
         <v>77</v>
       </c>
-      <c r="J91" s="145"/>
+      <c r="J91" s="147"/>
     </row>
     <row r="92" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B92" s="52"/>
@@ -4765,18 +4766,21 @@
       <c r="J121" s="101"/>
     </row>
     <row r="122" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B122" s="137"/>
-      <c r="C122" s="137"/>
-      <c r="D122" s="137"/>
-      <c r="E122" s="137"/>
-      <c r="F122" s="137"/>
-      <c r="G122" s="137"/>
-      <c r="H122" s="137"/>
-      <c r="I122" s="137"/>
-      <c r="J122" s="137"/>
+      <c r="B122" s="139"/>
+      <c r="C122" s="139"/>
+      <c r="D122" s="139"/>
+      <c r="E122" s="139"/>
+      <c r="F122" s="139"/>
+      <c r="G122" s="139"/>
+      <c r="H122" s="139"/>
+      <c r="I122" s="139"/>
+      <c r="J122" s="139"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="H72:J72"/>
+    <mergeCell ref="C73:G73"/>
+    <mergeCell ref="H73:J73"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="H5:J5"/>
     <mergeCell ref="D6:F6"/>
@@ -4793,9 +4797,6 @@
     <mergeCell ref="J78:K78"/>
     <mergeCell ref="C70:I70"/>
     <mergeCell ref="C72:G72"/>
-    <mergeCell ref="H72:J72"/>
-    <mergeCell ref="C73:G73"/>
-    <mergeCell ref="H73:J73"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="90" fitToHeight="2" orientation="portrait" r:id="rId1"/>
@@ -5461,15 +5462,15 @@
   <sheetData>
     <row r="1" spans="2:11" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:11" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="127" t="s">
+      <c r="C2" s="135" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="127"/>
-      <c r="E2" s="127"/>
-      <c r="F2" s="127"/>
-      <c r="G2" s="127"/>
-      <c r="H2" s="127"/>
-      <c r="I2" s="127"/>
+      <c r="D2" s="135"/>
+      <c r="E2" s="135"/>
+      <c r="F2" s="135"/>
+      <c r="G2" s="135"/>
+      <c r="H2" s="135"/>
+      <c r="I2" s="135"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
@@ -5487,39 +5488,39 @@
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C4" s="128" t="s">
+      <c r="C4" s="136" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="128"/>
-      <c r="E4" s="128"/>
-      <c r="F4" s="128"/>
-      <c r="G4" s="128"/>
-      <c r="H4" s="128"/>
-      <c r="I4" s="128"/>
-      <c r="J4" s="128"/>
+      <c r="D4" s="136"/>
+      <c r="E4" s="136"/>
+      <c r="F4" s="136"/>
+      <c r="G4" s="136"/>
+      <c r="H4" s="136"/>
+      <c r="I4" s="136"/>
+      <c r="J4" s="136"/>
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C5" s="128" t="s">
+      <c r="C5" s="136" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="128"/>
-      <c r="E5" s="128"/>
-      <c r="F5" s="128"/>
-      <c r="G5" s="128"/>
-      <c r="H5" s="126"/>
-      <c r="I5" s="126"/>
-      <c r="J5" s="126"/>
+      <c r="D5" s="136"/>
+      <c r="E5" s="136"/>
+      <c r="F5" s="136"/>
+      <c r="G5" s="136"/>
+      <c r="H5" s="134"/>
+      <c r="I5" s="134"/>
+      <c r="J5" s="134"/>
       <c r="K5" s="3"/>
     </row>
     <row r="6" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
-      <c r="D6" s="125"/>
-      <c r="E6" s="125"/>
-      <c r="F6" s="125"/>
-      <c r="H6" s="126"/>
-      <c r="I6" s="126"/>
-      <c r="J6" s="126"/>
+      <c r="D6" s="133"/>
+      <c r="E6" s="133"/>
+      <c r="F6" s="133"/>
+      <c r="H6" s="134"/>
+      <c r="I6" s="134"/>
+      <c r="J6" s="134"/>
       <c r="K6" s="3"/>
     </row>
     <row r="7" spans="2:11" ht="9.6" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5553,10 +5554,10 @@
       <c r="I10" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="J10" s="129">
+      <c r="J10" s="125">
         <v>45107</v>
       </c>
-      <c r="K10" s="129"/>
+      <c r="K10" s="125"/>
     </row>
     <row r="11" spans="2:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B11" s="8"/>
@@ -5685,24 +5686,24 @@
     </row>
     <row r="24" spans="2:17" ht="10.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="2:17" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B25" s="130" t="s">
+      <c r="B25" s="126" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="130"/>
-      <c r="D25" s="130"/>
-      <c r="E25" s="131"/>
-      <c r="F25" s="132" t="s">
+      <c r="C25" s="126"/>
+      <c r="D25" s="126"/>
+      <c r="E25" s="127"/>
+      <c r="F25" s="128" t="s">
         <v>25</v>
       </c>
-      <c r="G25" s="131"/>
-      <c r="H25" s="133" t="s">
+      <c r="G25" s="127"/>
+      <c r="H25" s="129" t="s">
         <v>26</v>
       </c>
-      <c r="I25" s="134"/>
-      <c r="J25" s="135" t="s">
+      <c r="I25" s="130"/>
+      <c r="J25" s="131" t="s">
         <v>12</v>
       </c>
-      <c r="K25" s="136"/>
+      <c r="K25" s="132"/>
     </row>
     <row r="26" spans="2:17" ht="13.9" x14ac:dyDescent="0.4">
       <c r="B26" s="37" t="s">
@@ -6129,17 +6130,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="J25:K25"/>
     <mergeCell ref="D6:F6"/>
     <mergeCell ref="H6:J6"/>
     <mergeCell ref="C2:I2"/>
     <mergeCell ref="C4:J4"/>
     <mergeCell ref="C5:G5"/>
     <mergeCell ref="H5:J5"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J25:K25"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="93" orientation="portrait" r:id="rId1"/>
@@ -6805,15 +6806,15 @@
   <sheetData>
     <row r="1" spans="2:11" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:11" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="127" t="s">
+      <c r="C2" s="135" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="127"/>
-      <c r="E2" s="127"/>
-      <c r="F2" s="127"/>
-      <c r="G2" s="127"/>
-      <c r="H2" s="127"/>
-      <c r="I2" s="127"/>
+      <c r="D2" s="135"/>
+      <c r="E2" s="135"/>
+      <c r="F2" s="135"/>
+      <c r="G2" s="135"/>
+      <c r="H2" s="135"/>
+      <c r="I2" s="135"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
@@ -6831,39 +6832,39 @@
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C4" s="128" t="s">
+      <c r="C4" s="136" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="128"/>
-      <c r="E4" s="128"/>
-      <c r="F4" s="128"/>
-      <c r="G4" s="128"/>
-      <c r="H4" s="128"/>
-      <c r="I4" s="128"/>
-      <c r="J4" s="128"/>
+      <c r="D4" s="136"/>
+      <c r="E4" s="136"/>
+      <c r="F4" s="136"/>
+      <c r="G4" s="136"/>
+      <c r="H4" s="136"/>
+      <c r="I4" s="136"/>
+      <c r="J4" s="136"/>
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C5" s="128" t="s">
+      <c r="C5" s="136" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="128"/>
-      <c r="E5" s="128"/>
-      <c r="F5" s="128"/>
-      <c r="G5" s="128"/>
-      <c r="H5" s="126"/>
-      <c r="I5" s="126"/>
-      <c r="J5" s="126"/>
+      <c r="D5" s="136"/>
+      <c r="E5" s="136"/>
+      <c r="F5" s="136"/>
+      <c r="G5" s="136"/>
+      <c r="H5" s="134"/>
+      <c r="I5" s="134"/>
+      <c r="J5" s="134"/>
       <c r="K5" s="3"/>
     </row>
     <row r="6" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
-      <c r="D6" s="125"/>
-      <c r="E6" s="125"/>
-      <c r="F6" s="125"/>
-      <c r="H6" s="126"/>
-      <c r="I6" s="126"/>
-      <c r="J6" s="126"/>
+      <c r="D6" s="133"/>
+      <c r="E6" s="133"/>
+      <c r="F6" s="133"/>
+      <c r="H6" s="134"/>
+      <c r="I6" s="134"/>
+      <c r="J6" s="134"/>
       <c r="K6" s="3"/>
     </row>
     <row r="7" spans="2:11" ht="9.6" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6897,10 +6898,10 @@
       <c r="I10" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="J10" s="129">
+      <c r="J10" s="125">
         <v>45079</v>
       </c>
-      <c r="K10" s="129"/>
+      <c r="K10" s="125"/>
     </row>
     <row r="11" spans="2:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B11" s="8"/>
@@ -7029,20 +7030,20 @@
     </row>
     <row r="24" spans="2:17" ht="10.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="2:17" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B25" s="130" t="s">
+      <c r="B25" s="126" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="130"/>
-      <c r="D25" s="130"/>
-      <c r="E25" s="131"/>
-      <c r="F25" s="141" t="s">
+      <c r="C25" s="126"/>
+      <c r="D25" s="126"/>
+      <c r="E25" s="127"/>
+      <c r="F25" s="143" t="s">
         <v>23</v>
       </c>
       <c r="G25" s="153"/>
-      <c r="H25" s="135" t="s">
+      <c r="H25" s="131" t="s">
         <v>12</v>
       </c>
-      <c r="I25" s="140"/>
+      <c r="I25" s="142"/>
     </row>
     <row r="26" spans="2:17" ht="13.9" x14ac:dyDescent="0.4">
       <c r="B26" s="37" t="s">

</xml_diff>

<commit_message>
empty assortiment bug fixed, working on empty rows table bug
</commit_message>
<xml_diff>
--- a/templates/KTI_Discharge_Invoice.xlsx
+++ b/templates/KTI_Discharge_Invoice.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B19E45-A9FE-455D-A351-085F60A589E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12076D56-8082-4F54-9E5E-6B2BD3FA5D4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26978" yWindow="-98" windowWidth="27076" windowHeight="16395" tabRatio="896" activeTab="1" xr2:uid="{A5E11D55-FD63-4C1B-A2BC-73BE53B894FE}"/>
+    <workbookView minimized="1" xWindow="-23250" yWindow="3112" windowWidth="14385" windowHeight="7486" tabRatio="896" activeTab="1" xr2:uid="{A5E11D55-FD63-4C1B-A2BC-73BE53B894FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Б.Нагаева хранение ТРК" sheetId="71" r:id="rId1"/>
@@ -1005,6 +1005,16 @@
     <xf numFmtId="169" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1029,16 +1039,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1079,10 +1083,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2380,15 +2380,15 @@
   <sheetData>
     <row r="1" spans="2:11" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:11" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="135" t="s">
+      <c r="C2" s="127" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="135"/>
-      <c r="E2" s="135"/>
-      <c r="F2" s="135"/>
-      <c r="G2" s="135"/>
-      <c r="H2" s="135"/>
-      <c r="I2" s="135"/>
+      <c r="D2" s="127"/>
+      <c r="E2" s="127"/>
+      <c r="F2" s="127"/>
+      <c r="G2" s="127"/>
+      <c r="H2" s="127"/>
+      <c r="I2" s="127"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
@@ -2406,39 +2406,39 @@
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C4" s="136" t="s">
+      <c r="C4" s="128" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="136"/>
-      <c r="E4" s="136"/>
-      <c r="F4" s="136"/>
-      <c r="G4" s="136"/>
-      <c r="H4" s="136"/>
-      <c r="I4" s="136"/>
-      <c r="J4" s="136"/>
+      <c r="D4" s="128"/>
+      <c r="E4" s="128"/>
+      <c r="F4" s="128"/>
+      <c r="G4" s="128"/>
+      <c r="H4" s="128"/>
+      <c r="I4" s="128"/>
+      <c r="J4" s="128"/>
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C5" s="136" t="s">
+      <c r="C5" s="128" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="136"/>
-      <c r="E5" s="136"/>
-      <c r="F5" s="136"/>
-      <c r="G5" s="136"/>
-      <c r="H5" s="134"/>
-      <c r="I5" s="134"/>
-      <c r="J5" s="134"/>
+      <c r="D5" s="128"/>
+      <c r="E5" s="128"/>
+      <c r="F5" s="128"/>
+      <c r="G5" s="128"/>
+      <c r="H5" s="126"/>
+      <c r="I5" s="126"/>
+      <c r="J5" s="126"/>
       <c r="K5" s="3"/>
     </row>
     <row r="6" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
-      <c r="D6" s="133"/>
-      <c r="E6" s="133"/>
-      <c r="F6" s="133"/>
-      <c r="H6" s="134"/>
-      <c r="I6" s="134"/>
-      <c r="J6" s="134"/>
+      <c r="D6" s="125"/>
+      <c r="E6" s="125"/>
+      <c r="F6" s="125"/>
+      <c r="H6" s="126"/>
+      <c r="I6" s="126"/>
+      <c r="J6" s="126"/>
       <c r="K6" s="3"/>
     </row>
     <row r="7" spans="2:11" ht="9.6" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2472,10 +2472,10 @@
       <c r="I10" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="J10" s="125">
+      <c r="J10" s="129">
         <v>45107</v>
       </c>
-      <c r="K10" s="125"/>
+      <c r="K10" s="129"/>
     </row>
     <row r="11" spans="2:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B11" s="8"/>
@@ -2604,24 +2604,24 @@
     </row>
     <row r="24" spans="2:17" ht="10.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="2:17" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B25" s="126" t="s">
+      <c r="B25" s="130" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="126"/>
-      <c r="D25" s="126"/>
-      <c r="E25" s="127"/>
-      <c r="F25" s="128" t="s">
+      <c r="C25" s="130"/>
+      <c r="D25" s="130"/>
+      <c r="E25" s="131"/>
+      <c r="F25" s="132" t="s">
         <v>25</v>
       </c>
-      <c r="G25" s="127"/>
-      <c r="H25" s="129" t="s">
+      <c r="G25" s="131"/>
+      <c r="H25" s="133" t="s">
         <v>26</v>
       </c>
-      <c r="I25" s="130"/>
-      <c r="J25" s="131" t="s">
+      <c r="I25" s="134"/>
+      <c r="J25" s="135" t="s">
         <v>12</v>
       </c>
-      <c r="K25" s="132"/>
+      <c r="K25" s="136"/>
     </row>
     <row r="26" spans="2:17" ht="13.9" x14ac:dyDescent="0.4">
       <c r="B26" s="37" t="s">
@@ -2996,17 +2996,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J25:K25"/>
     <mergeCell ref="D6:F6"/>
     <mergeCell ref="H6:J6"/>
     <mergeCell ref="C2:I2"/>
     <mergeCell ref="C4:J4"/>
     <mergeCell ref="C5:G5"/>
     <mergeCell ref="H5:J5"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="J25:K25"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="94" orientation="portrait" r:id="rId1"/>
@@ -3026,8 +3026,8 @@
   </sheetPr>
   <dimension ref="B1:Q122"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A63" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="J75" sqref="J75"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A11" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25:F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -3897,19 +3897,19 @@
       <c r="C5" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="137"/>
-      <c r="I5" s="137"/>
-      <c r="J5" s="137"/>
+      <c r="H5" s="139"/>
+      <c r="I5" s="139"/>
+      <c r="J5" s="139"/>
       <c r="K5" s="63"/>
     </row>
     <row r="6" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="63"/>
-      <c r="D6" s="138"/>
-      <c r="E6" s="138"/>
-      <c r="F6" s="138"/>
-      <c r="H6" s="137"/>
-      <c r="I6" s="137"/>
-      <c r="J6" s="137"/>
+      <c r="D6" s="140"/>
+      <c r="E6" s="140"/>
+      <c r="F6" s="140"/>
+      <c r="H6" s="139"/>
+      <c r="I6" s="139"/>
+      <c r="J6" s="139"/>
       <c r="K6" s="63"/>
     </row>
     <row r="7" spans="2:11" ht="9.6" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -3943,10 +3943,10 @@
       <c r="I10" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="J10" s="125">
+      <c r="J10" s="129">
         <v>45079</v>
       </c>
-      <c r="K10" s="125"/>
+      <c r="K10" s="129"/>
     </row>
     <row r="11" spans="2:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B11" s="8"/>
@@ -4061,21 +4061,21 @@
     </row>
     <row r="23" spans="2:17" ht="10.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="24" spans="2:17" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B24" s="140" t="s">
+      <c r="B24" s="142" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="140"/>
-      <c r="D24" s="140"/>
-      <c r="E24" s="140"/>
-      <c r="F24" s="141"/>
-      <c r="G24" s="143" t="s">
+      <c r="C24" s="142"/>
+      <c r="D24" s="142"/>
+      <c r="E24" s="142"/>
+      <c r="F24" s="143"/>
+      <c r="G24" s="145" t="s">
         <v>23</v>
       </c>
-      <c r="H24" s="140"/>
-      <c r="I24" s="131" t="s">
+      <c r="H24" s="142"/>
+      <c r="I24" s="135" t="s">
         <v>12</v>
       </c>
-      <c r="J24" s="142"/>
+      <c r="J24" s="144"/>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B25" s="10"/>
@@ -4281,15 +4281,15 @@
       <c r="I46" s="69"/>
     </row>
     <row r="70" spans="2:11" ht="30.4" x14ac:dyDescent="0.4">
-      <c r="C70" s="150" t="s">
+      <c r="C70" s="152" t="s">
         <v>46</v>
       </c>
-      <c r="D70" s="150"/>
-      <c r="E70" s="150"/>
-      <c r="F70" s="150"/>
-      <c r="G70" s="150"/>
-      <c r="H70" s="150"/>
-      <c r="I70" s="150"/>
+      <c r="D70" s="152"/>
+      <c r="E70" s="152"/>
+      <c r="F70" s="152"/>
+      <c r="G70" s="152"/>
+      <c r="H70" s="152"/>
+      <c r="I70" s="152"/>
       <c r="J70" s="61"/>
       <c r="K70" s="61"/>
     </row>
@@ -4307,44 +4307,44 @@
       <c r="K71" s="94"/>
     </row>
     <row r="72" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="C72" s="151" t="s">
+      <c r="C72" s="138" t="s">
         <v>48</v>
       </c>
-      <c r="D72" s="151"/>
-      <c r="E72" s="151"/>
-      <c r="F72" s="151"/>
-      <c r="G72" s="151"/>
-      <c r="H72" s="152"/>
-      <c r="I72" s="152"/>
-      <c r="J72" s="152"/>
+      <c r="D72" s="138"/>
+      <c r="E72" s="138"/>
+      <c r="F72" s="138"/>
+      <c r="G72" s="138"/>
+      <c r="H72" s="137"/>
+      <c r="I72" s="137"/>
+      <c r="J72" s="137"/>
       <c r="K72" s="95"/>
     </row>
     <row r="73" spans="2:11" ht="15" x14ac:dyDescent="0.4">
       <c r="B73" s="63"/>
-      <c r="C73" s="151" t="s">
+      <c r="C73" s="138" t="s">
         <v>49</v>
       </c>
-      <c r="D73" s="151"/>
-      <c r="E73" s="151"/>
-      <c r="F73" s="151"/>
-      <c r="G73" s="151"/>
-      <c r="H73" s="152"/>
-      <c r="I73" s="152"/>
-      <c r="J73" s="152"/>
+      <c r="D73" s="138"/>
+      <c r="E73" s="138"/>
+      <c r="F73" s="138"/>
+      <c r="G73" s="138"/>
+      <c r="H73" s="137"/>
+      <c r="I73" s="137"/>
+      <c r="J73" s="137"/>
       <c r="K73" s="95"/>
     </row>
     <row r="74" spans="2:11" ht="15" x14ac:dyDescent="0.4">
       <c r="B74" s="63"/>
-      <c r="C74" s="136" t="s">
+      <c r="C74" s="128" t="s">
         <v>3</v>
       </c>
-      <c r="D74" s="136"/>
-      <c r="E74" s="136"/>
-      <c r="F74" s="136"/>
-      <c r="G74" s="136"/>
-      <c r="H74" s="137"/>
-      <c r="I74" s="137"/>
-      <c r="J74" s="137"/>
+      <c r="D74" s="128"/>
+      <c r="E74" s="128"/>
+      <c r="F74" s="128"/>
+      <c r="G74" s="128"/>
+      <c r="H74" s="139"/>
+      <c r="I74" s="139"/>
+      <c r="J74" s="139"/>
       <c r="K74" s="63"/>
     </row>
     <row r="76" spans="2:11" ht="15" x14ac:dyDescent="0.4">
@@ -4376,10 +4376,10 @@
       <c r="I78" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="J78" s="149">
+      <c r="J78" s="151">
         <v>45033</v>
       </c>
-      <c r="K78" s="149"/>
+      <c r="K78" s="151"/>
     </row>
     <row r="79" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B79" s="8"/>
@@ -4498,21 +4498,21 @@
       <c r="J90" s="121"/>
     </row>
     <row r="91" spans="2:11" ht="19.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B91" s="144" t="s">
+      <c r="B91" s="146" t="s">
         <v>75</v>
       </c>
-      <c r="C91" s="144"/>
-      <c r="D91" s="144"/>
-      <c r="E91" s="144"/>
-      <c r="F91" s="145"/>
-      <c r="G91" s="146" t="s">
+      <c r="C91" s="146"/>
+      <c r="D91" s="146"/>
+      <c r="E91" s="146"/>
+      <c r="F91" s="147"/>
+      <c r="G91" s="148" t="s">
         <v>76</v>
       </c>
-      <c r="H91" s="148"/>
-      <c r="I91" s="146" t="s">
+      <c r="H91" s="150"/>
+      <c r="I91" s="148" t="s">
         <v>77</v>
       </c>
-      <c r="J91" s="147"/>
+      <c r="J91" s="149"/>
     </row>
     <row r="92" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B92" s="52"/>
@@ -4766,25 +4766,18 @@
       <c r="J121" s="101"/>
     </row>
     <row r="122" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B122" s="139"/>
-      <c r="C122" s="139"/>
-      <c r="D122" s="139"/>
-      <c r="E122" s="139"/>
-      <c r="F122" s="139"/>
-      <c r="G122" s="139"/>
-      <c r="H122" s="139"/>
-      <c r="I122" s="139"/>
-      <c r="J122" s="139"/>
+      <c r="B122" s="141"/>
+      <c r="C122" s="141"/>
+      <c r="D122" s="141"/>
+      <c r="E122" s="141"/>
+      <c r="F122" s="141"/>
+      <c r="G122" s="141"/>
+      <c r="H122" s="141"/>
+      <c r="I122" s="141"/>
+      <c r="J122" s="141"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="H72:J72"/>
-    <mergeCell ref="C73:G73"/>
-    <mergeCell ref="H73:J73"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="H6:J6"/>
     <mergeCell ref="B122:J122"/>
     <mergeCell ref="B24:F24"/>
     <mergeCell ref="I24:J24"/>
@@ -4797,6 +4790,13 @@
     <mergeCell ref="J78:K78"/>
     <mergeCell ref="C70:I70"/>
     <mergeCell ref="C72:G72"/>
+    <mergeCell ref="H72:J72"/>
+    <mergeCell ref="C73:G73"/>
+    <mergeCell ref="H73:J73"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="H6:J6"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="90" fitToHeight="2" orientation="portrait" r:id="rId1"/>
@@ -5462,15 +5462,15 @@
   <sheetData>
     <row r="1" spans="2:11" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:11" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="135" t="s">
+      <c r="C2" s="127" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="135"/>
-      <c r="E2" s="135"/>
-      <c r="F2" s="135"/>
-      <c r="G2" s="135"/>
-      <c r="H2" s="135"/>
-      <c r="I2" s="135"/>
+      <c r="D2" s="127"/>
+      <c r="E2" s="127"/>
+      <c r="F2" s="127"/>
+      <c r="G2" s="127"/>
+      <c r="H2" s="127"/>
+      <c r="I2" s="127"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
@@ -5488,39 +5488,39 @@
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C4" s="136" t="s">
+      <c r="C4" s="128" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="136"/>
-      <c r="E4" s="136"/>
-      <c r="F4" s="136"/>
-      <c r="G4" s="136"/>
-      <c r="H4" s="136"/>
-      <c r="I4" s="136"/>
-      <c r="J4" s="136"/>
+      <c r="D4" s="128"/>
+      <c r="E4" s="128"/>
+      <c r="F4" s="128"/>
+      <c r="G4" s="128"/>
+      <c r="H4" s="128"/>
+      <c r="I4" s="128"/>
+      <c r="J4" s="128"/>
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C5" s="136" t="s">
+      <c r="C5" s="128" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="136"/>
-      <c r="E5" s="136"/>
-      <c r="F5" s="136"/>
-      <c r="G5" s="136"/>
-      <c r="H5" s="134"/>
-      <c r="I5" s="134"/>
-      <c r="J5" s="134"/>
+      <c r="D5" s="128"/>
+      <c r="E5" s="128"/>
+      <c r="F5" s="128"/>
+      <c r="G5" s="128"/>
+      <c r="H5" s="126"/>
+      <c r="I5" s="126"/>
+      <c r="J5" s="126"/>
       <c r="K5" s="3"/>
     </row>
     <row r="6" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
-      <c r="D6" s="133"/>
-      <c r="E6" s="133"/>
-      <c r="F6" s="133"/>
-      <c r="H6" s="134"/>
-      <c r="I6" s="134"/>
-      <c r="J6" s="134"/>
+      <c r="D6" s="125"/>
+      <c r="E6" s="125"/>
+      <c r="F6" s="125"/>
+      <c r="H6" s="126"/>
+      <c r="I6" s="126"/>
+      <c r="J6" s="126"/>
       <c r="K6" s="3"/>
     </row>
     <row r="7" spans="2:11" ht="9.6" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5554,10 +5554,10 @@
       <c r="I10" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="J10" s="125">
+      <c r="J10" s="129">
         <v>45107</v>
       </c>
-      <c r="K10" s="125"/>
+      <c r="K10" s="129"/>
     </row>
     <row r="11" spans="2:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B11" s="8"/>
@@ -5686,24 +5686,24 @@
     </row>
     <row r="24" spans="2:17" ht="10.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="2:17" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B25" s="126" t="s">
+      <c r="B25" s="130" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="126"/>
-      <c r="D25" s="126"/>
-      <c r="E25" s="127"/>
-      <c r="F25" s="128" t="s">
+      <c r="C25" s="130"/>
+      <c r="D25" s="130"/>
+      <c r="E25" s="131"/>
+      <c r="F25" s="132" t="s">
         <v>25</v>
       </c>
-      <c r="G25" s="127"/>
-      <c r="H25" s="129" t="s">
+      <c r="G25" s="131"/>
+      <c r="H25" s="133" t="s">
         <v>26</v>
       </c>
-      <c r="I25" s="130"/>
-      <c r="J25" s="131" t="s">
+      <c r="I25" s="134"/>
+      <c r="J25" s="135" t="s">
         <v>12</v>
       </c>
-      <c r="K25" s="132"/>
+      <c r="K25" s="136"/>
     </row>
     <row r="26" spans="2:17" ht="13.9" x14ac:dyDescent="0.4">
       <c r="B26" s="37" t="s">
@@ -6130,17 +6130,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J25:K25"/>
     <mergeCell ref="D6:F6"/>
     <mergeCell ref="H6:J6"/>
     <mergeCell ref="C2:I2"/>
     <mergeCell ref="C4:J4"/>
     <mergeCell ref="C5:G5"/>
     <mergeCell ref="H5:J5"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="J25:K25"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="93" orientation="portrait" r:id="rId1"/>
@@ -6806,15 +6806,15 @@
   <sheetData>
     <row r="1" spans="2:11" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:11" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="135" t="s">
+      <c r="C2" s="127" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="135"/>
-      <c r="E2" s="135"/>
-      <c r="F2" s="135"/>
-      <c r="G2" s="135"/>
-      <c r="H2" s="135"/>
-      <c r="I2" s="135"/>
+      <c r="D2" s="127"/>
+      <c r="E2" s="127"/>
+      <c r="F2" s="127"/>
+      <c r="G2" s="127"/>
+      <c r="H2" s="127"/>
+      <c r="I2" s="127"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
@@ -6832,39 +6832,39 @@
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C4" s="136" t="s">
+      <c r="C4" s="128" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="136"/>
-      <c r="E4" s="136"/>
-      <c r="F4" s="136"/>
-      <c r="G4" s="136"/>
-      <c r="H4" s="136"/>
-      <c r="I4" s="136"/>
-      <c r="J4" s="136"/>
+      <c r="D4" s="128"/>
+      <c r="E4" s="128"/>
+      <c r="F4" s="128"/>
+      <c r="G4" s="128"/>
+      <c r="H4" s="128"/>
+      <c r="I4" s="128"/>
+      <c r="J4" s="128"/>
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C5" s="136" t="s">
+      <c r="C5" s="128" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="136"/>
-      <c r="E5" s="136"/>
-      <c r="F5" s="136"/>
-      <c r="G5" s="136"/>
-      <c r="H5" s="134"/>
-      <c r="I5" s="134"/>
-      <c r="J5" s="134"/>
+      <c r="D5" s="128"/>
+      <c r="E5" s="128"/>
+      <c r="F5" s="128"/>
+      <c r="G5" s="128"/>
+      <c r="H5" s="126"/>
+      <c r="I5" s="126"/>
+      <c r="J5" s="126"/>
       <c r="K5" s="3"/>
     </row>
     <row r="6" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
-      <c r="D6" s="133"/>
-      <c r="E6" s="133"/>
-      <c r="F6" s="133"/>
-      <c r="H6" s="134"/>
-      <c r="I6" s="134"/>
-      <c r="J6" s="134"/>
+      <c r="D6" s="125"/>
+      <c r="E6" s="125"/>
+      <c r="F6" s="125"/>
+      <c r="H6" s="126"/>
+      <c r="I6" s="126"/>
+      <c r="J6" s="126"/>
       <c r="K6" s="3"/>
     </row>
     <row r="7" spans="2:11" ht="9.6" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6898,10 +6898,10 @@
       <c r="I10" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="J10" s="125">
+      <c r="J10" s="129">
         <v>45079</v>
       </c>
-      <c r="K10" s="125"/>
+      <c r="K10" s="129"/>
     </row>
     <row r="11" spans="2:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B11" s="8"/>
@@ -7030,20 +7030,20 @@
     </row>
     <row r="24" spans="2:17" ht="10.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="2:17" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B25" s="126" t="s">
+      <c r="B25" s="130" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="126"/>
-      <c r="D25" s="126"/>
-      <c r="E25" s="127"/>
-      <c r="F25" s="143" t="s">
+      <c r="C25" s="130"/>
+      <c r="D25" s="130"/>
+      <c r="E25" s="131"/>
+      <c r="F25" s="145" t="s">
         <v>23</v>
       </c>
       <c r="G25" s="153"/>
-      <c r="H25" s="131" t="s">
+      <c r="H25" s="135" t="s">
         <v>12</v>
       </c>
-      <c r="I25" s="142"/>
+      <c r="I25" s="144"/>
     </row>
     <row r="26" spans="2:17" ht="13.9" x14ac:dyDescent="0.4">
       <c r="B26" s="37" t="s">

</xml_diff>